<commit_message>
Refactor documentation for Python in Excel use cases: - Update geospatial plots section to clarify library requirements and visualization capabilities. - Enhance reporting and automation guides with advanced techniques and further analysis sections. - Introduce user-defined functions (UDFs) with detailed examples for custom calculations in Excel. - Revise README for improved structure and clarity, adding use case categories and setup requirements.
</commit_message>
<xml_diff>
--- a/data/00-{Industry}_00-{UseCase}.xlsx
+++ b/data/00-{Industry}_00-{UseCase}.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01-Projects\PythonInExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01-Projects\PythonInExcel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390788F8-9C9B-417C-8CB0-A24D1A6AC93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BB579D-B3C9-4363-B019-C1E6FBE356DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{459F3AEC-747D-481E-9146-83D565F98550}"/>
+    <workbookView xWindow="-20625" yWindow="2940" windowWidth="11970" windowHeight="6000" activeTab="1" xr2:uid="{459F3AEC-747D-481E-9146-83D565F98550}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -913,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC99BF9-B482-440F-ADE2-523071E73D38}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,50 +944,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="str" cm="1">
-        <f t="array" ref="A7:F11">_xlfn._xlws.PY(1,0,TblName001[#All])</f>
+    <row r="8" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="str" cm="1">
+        <f t="array" ref="A8:F12">_xlfn._xlws.PY(1,0,TblName001[#All])</f>
         <v>Col1</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B8" t="str">
         <v>Col2</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C8" t="str">
         <v>Col3</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D8" t="str">
         <v>Col4</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E8" t="str">
         <v>Col5</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F8" t="str">
         <v>Col6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" vm="2">
-        <v>0</v>
-      </c>
-      <c r="B8" vm="2">
-        <v>0</v>
-      </c>
-      <c r="C8" vm="2">
-        <v>0</v>
-      </c>
-      <c r="D8" vm="2">
-        <v>0</v>
-      </c>
-      <c r="E8" vm="2">
-        <v>0</v>
-      </c>
-      <c r="F8" vm="2">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,61 +1030,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" vm="2">
+        <v>0</v>
+      </c>
+      <c r="B12" vm="2">
+        <v>0</v>
+      </c>
+      <c r="C12" vm="2">
+        <v>0</v>
+      </c>
+      <c r="D12" vm="2">
+        <v>0</v>
+      </c>
+      <c r="E12" vm="2">
+        <v>0</v>
+      </c>
+      <c r="F12" vm="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="e" cm="1" vm="3">
-        <f t="array" ref="A15">_xlfn._xlws.PY(2,1,TblName001[#All])</f>
+    <row r="16" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="e" cm="1" vm="3">
+        <f t="array" ref="A16">_xlfn._xlws.PY(2,1,TblName001[#All])</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="str" cm="1">
-        <f t="array" ref="A18:F22">_xlfn._xlws.PY(3,0)</f>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="str" cm="1">
+        <f t="array" ref="A19:F23">_xlfn._xlws.PY(3,0)</f>
         <v>Col1</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B19" t="str">
         <v>Col2</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C19" t="str">
         <v>Col3</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D19" t="str">
         <v>Col4</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E19" t="str">
         <v>Col5</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F19" t="str">
         <v>Col6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" vm="2">
-        <v>0</v>
-      </c>
-      <c r="B19" vm="2">
-        <v>0</v>
-      </c>
-      <c r="C19" vm="2">
-        <v>0</v>
-      </c>
-      <c r="D19" vm="2">
-        <v>0</v>
-      </c>
-      <c r="E19" vm="2">
-        <v>0</v>
-      </c>
-      <c r="F19" vm="2">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,23 +1147,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" vm="2">
+        <v>0</v>
+      </c>
+      <c r="B23" vm="2">
+        <v>0</v>
+      </c>
+      <c r="C23" vm="2">
+        <v>0</v>
+      </c>
+      <c r="D23" vm="2">
+        <v>0</v>
+      </c>
+      <c r="E23" vm="2">
+        <v>0</v>
+      </c>
+      <c r="F23" vm="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
@@ -1194,18 +1191,21 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
     </row>
-    <row r="66" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="67" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>